<commit_message>
edit the columns in import student template
</commit_message>
<xml_diff>
--- a/public/files/import_student_template.xlsx
+++ b/public/files/import_student_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://anasacademy-my.sharepoint.com/personal/eman_m_anasacademy_uk/Documents/Desktop/lms/public/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\lms\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{A5A76B7D-21E8-4306-9DBC-B14ED8793295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8862FB87-B6F0-45C8-A971-D13125F16551}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF6DD77-DA5B-45F8-AD75-7E2CAEEE4367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>الاسم ثلاثي باللغة العربية</t>
   </si>
@@ -34,88 +34,16 @@
     <t>رقم الجوال</t>
   </si>
   <si>
-    <t>رقم الهاتف</t>
-  </si>
-  <si>
     <t>رقم الهوية او جواز السفر</t>
   </si>
   <si>
-    <t>كود الدبلوم</t>
-  </si>
-  <si>
-    <t>الجنسية</t>
-  </si>
-  <si>
-    <t>الدولة</t>
-  </si>
-  <si>
-    <t>مدينة الاقامه</t>
-  </si>
-  <si>
-    <t>الجامعه</t>
-  </si>
-  <si>
-    <t>الكلية</t>
-  </si>
-  <si>
-    <t>التخصص التعليمي</t>
-  </si>
-  <si>
-    <t>سنة التخرج</t>
-  </si>
-  <si>
-    <t>المعدل/ التقدير الجامعي/ gpa</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> المدرسة</t>
-  </si>
-  <si>
-    <t>بلد مصدر شهادة البكالوريوس/الثانوية</t>
-  </si>
-  <si>
-    <t>معدل المرحلة الثانوية</t>
-  </si>
-  <si>
-    <t>سنة الحصول على الشهادة الثانوية</t>
-  </si>
-  <si>
     <t>من اين عرفت عن الاكاديمية</t>
   </si>
   <si>
-    <t>اسم شخص للتواصل معه عند الضرورة</t>
-  </si>
-  <si>
-    <t>البريد الالكتروني للشخص</t>
-  </si>
-  <si>
-    <t>رقم جوال الشخص</t>
-  </si>
-  <si>
-    <t xml:space="preserve">صلة القرابة للشخص </t>
-  </si>
-  <si>
-    <t>جهة العمل(حكومة/خاصة)</t>
-  </si>
-  <si>
-    <t>الوظيفة</t>
-  </si>
-  <si>
-    <t>المشكلة الصحية</t>
-  </si>
-  <si>
-    <t>نوع الإعاقة</t>
-  </si>
-  <si>
-    <t>هل أنت من الصم وضعاف السمع؟(نعم/لا)</t>
-  </si>
-  <si>
-    <t>المنطقة التعليمية ثانوي/بكالوريوس</t>
-  </si>
-  <si>
-    <t>تاريخ الميلاد(yyyy-mm-dd)</t>
-  </si>
-  <si>
     <t>الجنس(male/female)</t>
+  </si>
+  <si>
+    <t>كود البرنامج</t>
   </si>
 </sst>
 </file>
@@ -163,11 +91,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -481,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,34 +419,32 @@
     <col min="1" max="1" width="38.7109375" customWidth="1"/>
     <col min="2" max="3" width="24.42578125" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" customWidth="1"/>
-    <col min="13" max="13" width="31.42578125" customWidth="1"/>
-    <col min="14" max="14" width="41.42578125" customWidth="1"/>
-    <col min="15" max="15" width="21" customWidth="1"/>
-    <col min="16" max="16" width="24" customWidth="1"/>
-    <col min="17" max="17" width="28.5703125" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" customWidth="1"/>
-    <col min="19" max="19" width="27.28515625" customWidth="1"/>
-    <col min="20" max="20" width="19.28515625" customWidth="1"/>
-    <col min="21" max="21" width="22.7109375" customWidth="1"/>
-    <col min="22" max="23" width="35.7109375" customWidth="1"/>
-    <col min="24" max="24" width="17.85546875" customWidth="1"/>
-    <col min="25" max="25" width="26.140625" customWidth="1"/>
-    <col min="26" max="26" width="21.7109375" customWidth="1"/>
-    <col min="27" max="27" width="23.7109375" customWidth="1"/>
-    <col min="28" max="28" width="30.28515625" customWidth="1"/>
-    <col min="29" max="29" width="22.85546875" customWidth="1"/>
-    <col min="30" max="30" width="22.140625" customWidth="1"/>
-    <col min="31" max="31" width="18" customWidth="1"/>
-    <col min="32" max="32" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="31.42578125" customWidth="1"/>
+    <col min="12" max="12" width="41.42578125" customWidth="1"/>
+    <col min="13" max="13" width="21" customWidth="1"/>
+    <col min="14" max="14" width="24" customWidth="1"/>
+    <col min="15" max="15" width="28.5703125" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" customWidth="1"/>
+    <col min="17" max="17" width="27.28515625" customWidth="1"/>
+    <col min="18" max="18" width="19.28515625" customWidth="1"/>
+    <col min="19" max="19" width="22.7109375" customWidth="1"/>
+    <col min="20" max="20" width="35.7109375" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" customWidth="1"/>
+    <col min="22" max="22" width="26.140625" customWidth="1"/>
+    <col min="23" max="23" width="21.7109375" customWidth="1"/>
+    <col min="24" max="24" width="23.7109375" customWidth="1"/>
+    <col min="25" max="25" width="30.28515625" customWidth="1"/>
+    <col min="26" max="26" width="22.85546875" customWidth="1"/>
+    <col min="27" max="27" width="22.140625" customWidth="1"/>
+    <col min="28" max="28" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,95 +458,35 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
       <c r="G1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="L1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
-      <c r="F2" s="3"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -631,33 +496,9 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="2"/>
-      <c r="AF2" s="1"/>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="2"/>
-      <c r="AF3" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>